<commit_message>
ventana de login con hash antes de persistir.
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>anteproyecto</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>diseño ventana login - curso java sql Codigos de Programacion - conecto el proyecto con github</t>
+  </si>
+  <si>
+    <t>estudio db40 pero lo desecho finalmente, ya no existe. Inicio el programaa con la ventana de login en lugar de la principal</t>
+  </si>
+  <si>
+    <t>estudio ObjectDB - tutorial</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,6 +520,22 @@
       </c>
       <c r="B14" s="1">
         <v>44054</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>